<commit_message>
add new feature in example import
</commit_message>
<xml_diff>
--- a/artcoded/src/main/resources/dossier/import-dossier-example.xlsx
+++ b/artcoded/src/main/resources/dossier/import-dossier-example.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="86">
   <si>
     <t xml:space="preserve">Dossiers imported</t>
   </si>
@@ -53,7 +53,7 @@
     <t xml:space="preserve">This feature is experimental! We create a backup before importing the dossier(s), in order to rollback in case an error occurs.</t>
   </si>
   <si>
-    <t xml:space="preserve">This is an example sheet, don't forget to remove the example rows</t>
+    <t xml:space="preserve">This is an example sheet, don't forget to remove the example rows.</t>
   </si>
   <si>
     <t xml:space="preserve">How To</t>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t xml:space="preserve">KEEP THE HEADER (title) on each tab!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Feature: you can specify multiple file names for expense, just separate them with a ","</t>
   </si>
   <si>
     <t xml:space="preserve">Name</t>
@@ -289,7 +292,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -313,13 +316,20 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FFCCCCCC"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -330,6 +340,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00A933"/>
+        <bgColor rgb="FF008000"/>
       </patternFill>
     </fill>
   </fills>
@@ -367,7 +383,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -380,7 +396,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -397,6 +417,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFCCCCCC"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF00A933"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -405,13 +485,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A22"/>
+  <dimension ref="A1:A25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="108.8"/>
   </cols>
@@ -466,49 +546,54 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -533,7 +618,7 @@
       <selection pane="topLeft" activeCell="J6" activeCellId="0" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="16.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="23.48"/>
@@ -546,69 +631,69 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="B2" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="C2" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="G2" s="5" t="s">
         <v>38</v>
       </c>
+      <c r="H2" s="5" t="s">
+        <v>39</v>
+      </c>
       <c r="I2" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J2" s="2" t="n">
         <v>30</v>
@@ -617,36 +702,36 @@
         <v>450</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G3" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="G3" s="5" t="s">
         <v>48</v>
       </c>
+      <c r="H3" s="5" t="s">
+        <v>49</v>
+      </c>
       <c r="I3" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J3" s="2" t="n">
         <v>30</v>
@@ -655,7 +740,7 @@
         <v>500</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -680,48 +765,48 @@
       <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>52</v>
+      <c r="B2" s="5" t="s">
+        <v>53</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>53</v>
+      <c r="D2" s="5" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>54</v>
+      <c r="B3" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>55</v>
+      <c r="D3" s="5" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -746,7 +831,7 @@
       <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="19.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="2" width="17.78"/>
@@ -757,51 +842,51 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
-        <v>65</v>
+      <c r="A2" s="5" t="s">
+        <v>66</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C2" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>68</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>69</v>
       </c>
       <c r="E2" s="2" t="n">
         <v>21</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G2" s="2" t="n">
         <v>15</v>
@@ -810,27 +895,27 @@
         <v>1</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
-        <v>70</v>
+      <c r="A3" s="5" t="s">
+        <v>71</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D3" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>72</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>73</v>
       </c>
       <c r="E3" s="2" t="n">
         <v>21</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G3" s="2" t="n">
         <v>15</v>
@@ -839,7 +924,7 @@
         <v>5</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -864,7 +949,7 @@
       <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="26.95"/>
@@ -875,48 +960,48 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C2" s="4" t="s">
         <v>79</v>
       </c>
+      <c r="C2" s="5" t="s">
+        <v>80</v>
+      </c>
       <c r="D2" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G2" s="2" t="n">
         <v>100</v>
@@ -927,22 +1012,22 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C3" s="4" t="s">
         <v>83</v>
       </c>
+      <c r="C3" s="5" t="s">
+        <v>84</v>
+      </c>
       <c r="D3" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G3" s="2" t="n">
         <v>100</v>

</xml_diff>